<commit_message>
Updated samples with more tests
</commit_message>
<xml_diff>
--- a/basics/optional_arguments.xlsx
+++ b/basics/optional_arguments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDB0138-DF57-4E16-A65F-D1243CC32C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12157A56-B614-4192-9F1D-416724E2D364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{C920AF47-D7E2-43A0-A8C9-A41258185E24}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>One</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>This is mainly a test workbook to show that missing optional arguments are correcty detected and defaulted</t>
+  </si>
+  <si>
+    <t>Optional Arg Value</t>
   </si>
 </sst>
 </file>
@@ -550,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999D0D9F-3C3C-48A8-86D4-0518FA0E9B38}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -561,9 +564,10 @@
     <col min="1" max="1" width="21.15234375" customWidth="1"/>
     <col min="2" max="2" width="20.765625" customWidth="1"/>
     <col min="3" max="3" width="16.765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -572,7 +576,7 @@
         <v>D:\github\xlslim-code-samples\basics</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -581,16 +585,16 @@
         <v>D:\github\xlslim-code-samples\basics\optional_arguments.py</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" ref="B3">_xll.RegisterPyModule(B2)</f>
-        <v>Registered D:\github\xlslim-code-samples\basics\optional_arguments.py</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+        <v>Initialised the Python environment at C:\Users\russe\AppData\Local\Programs\Python\Python312\xlslim. Registered D:\github\xlslim-code-samples\basics\optional_arguments.py</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -600,8 +604,14 @@
       <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -610,14 +620,18 @@
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="2" t="e" cm="1">
+        <f t="array" ref="D6">_xll.echo_default(A6)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -629,12 +643,20 @@
         <f t="array" ref="C7">_xll.echo_type_int_list(A7)</f>
         <v>&lt;class 'list'&gt;</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D7" s="2" cm="1">
+        <f t="array" ref="D7">_xll.echo_int(A7)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" cm="1">
+        <f t="array" ref="E7">_xll.echo_int_list(A7)</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -646,12 +668,20 @@
         <f t="array" ref="C8">_xll.echo_type_int_list_none(A8)</f>
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D8" s="2" t="e" cm="1">
+        <f t="array" ref="D8">_xll.echo_int_none(A8)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E8" s="2" t="e" cm="1">
+        <f t="array" ref="E8">_xll.echo_int_list_none(A8)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -663,8 +693,16 @@
         <f t="array" ref="C9">_xll.echo_type_optional_int_list(A9)</f>
         <v>&lt;class 'list'&gt;</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D9" s="2" cm="1">
+        <f t="array" ref="D9">_xll.echo_optional_int(A9)</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" cm="1">
+        <f t="array" ref="E9">_xll.echo_optional_int_list(A9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -676,8 +714,16 @@
         <f t="array" ref="C10">_xll.echo_type_optional_int_list_none(A10)</f>
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D10" s="2" t="e" cm="1">
+        <f t="array" ref="D10">_xll.echo_optional_int_none(A10)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E10" s="2" t="e" cm="1">
+        <f t="array" ref="E10">_xll.echo_optional_int_list_none(A10)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -689,8 +735,16 @@
         <f t="array" ref="C11">_xll.echo_type_float_list(A11)</f>
         <v>&lt;class 'list'&gt;</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D11" s="2" cm="1">
+        <f t="array" ref="D11">_xll.echo_float(A11)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="e" cm="1">
+        <f t="array" ref="E11">_xll.echo_float_list(A11)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -702,8 +756,16 @@
         <f t="array" ref="C12">_xll.echo_type_float_list_none(A12)</f>
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D12" s="2" t="str" cm="1">
+        <f t="array" ref="D12">_xll.echo_float_none(A12)</f>
+        <v>#ERR The function call failed - 'NoneType' object has no attribute '__float__'</v>
+      </c>
+      <c r="E12" s="2" t="e" cm="1">
+        <f t="array" ref="E12">_xll.echo_float_list_none(A12)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -715,8 +777,16 @@
         <f t="array" ref="C13">_xll.echo_type_optional_float_list(A13)</f>
         <v>&lt;class 'list'&gt;</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D13" s="2" cm="1">
+        <f t="array" ref="D13">_xll.echo_optional_float(A13)</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="E13" s="2" t="e" cm="1">
+        <f t="array" ref="E13">_xll.echo_optional_float_list(A13)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="4">
         <v>1</v>
       </c>
@@ -728,8 +798,16 @@
         <f t="array" ref="C14">_xll.echo_type_optional_float_list_none(A14)</f>
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D14" s="2" t="str" cm="1">
+        <f t="array" ref="D14">_xll.echo_optional_float_none(A14)</f>
+        <v>#ERR The function call failed - 'NoneType' object has no attribute '__float__'</v>
+      </c>
+      <c r="E14" s="2" t="e" cm="1">
+        <f t="array" ref="E14">_xll.echo_optional_float_list_none(A14)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="b">
         <v>1</v>
       </c>
@@ -741,8 +819,16 @@
         <f t="array" ref="C15">_xll.echo_type_bool_list(A15)</f>
         <v>&lt;class 'list'&gt;</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D15" s="2" t="b" cm="1">
+        <f t="array" ref="D15">_xll.echo_bool(A15)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="b" cm="1">
+        <f t="array" ref="E15">_xll.echo_bool_list(A15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="b">
         <v>1</v>
       </c>
@@ -754,8 +840,16 @@
         <f t="array" ref="C16">_xll.echo_type_bool_list_none(A16)</f>
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D16" s="2" t="e" cm="1">
+        <f t="array" ref="D16">_xll.echo_bool_none(A16)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E16" s="2" t="e" cm="1">
+        <f t="array" ref="E16">_xll.echo_bool_list_none(A16)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="b">
         <v>1</v>
       </c>
@@ -767,8 +861,16 @@
         <f t="array" ref="C17">_xll.echo_type_optional_bool_list(A17)</f>
         <v>&lt;class 'list'&gt;</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D17" s="2" t="b" cm="1">
+        <f t="array" ref="D17">_xll.echo_optional_bool(A17)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="b" cm="1">
+        <f t="array" ref="E17">_xll.echo_optional_bool_list(A17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="b">
         <v>1</v>
       </c>
@@ -780,8 +882,16 @@
         <f t="array" ref="C18">_xll.echo_type_optional_bool_list_none(A18)</f>
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D18" s="2" t="e" cm="1">
+        <f t="array" ref="D18">_xll.echo_optional_bool_none(A18)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E18" s="2" t="e" cm="1">
+        <f t="array" ref="E18">_xll.echo_optional_bool_list_none(A18)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>0</v>
       </c>
@@ -793,8 +903,16 @@
         <f t="array" ref="C19">_xll.echo_type_str_list(A19)</f>
         <v>&lt;class 'list'&gt;</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D19" s="2" t="str" cm="1">
+        <f t="array" ref="D19">_xll.echo_str(A19)</f>
+        <v>test</v>
+      </c>
+      <c r="E19" s="2" t="str" cm="1">
+        <f t="array" ref="E19">_xll.echo_str_list(A19)</f>
+        <v>test</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
@@ -806,8 +924,16 @@
         <f t="array" ref="C20">_xll.echo_type_str_list_none(A20)</f>
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D20" s="2" t="e" cm="1">
+        <f t="array" ref="D20">_xll.echo_str_none(A20)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E20" s="2" t="e" cm="1">
+        <f t="array" ref="E20">_xll.echo_str_list_none(A20)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>0</v>
       </c>
@@ -819,8 +945,16 @@
         <f t="array" ref="C21">_xll.echo_type_optional_str_list(A21)</f>
         <v>&lt;class 'list'&gt;</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D21" s="2" t="str" cm="1">
+        <f t="array" ref="D21">_xll.echo_optional_str(A21)</f>
+        <v>test</v>
+      </c>
+      <c r="E21" s="2" t="str" cm="1">
+        <f t="array" ref="E21">_xll.echo_optional_str_list(A21)</f>
+        <v>test</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>0</v>
       </c>
@@ -832,11 +966,19 @@
         <f t="array" ref="C22">_xll.echo_type_optional_str_list_none(A22)</f>
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D22" s="2" t="e" cm="1">
+        <f t="array" ref="D22">_xll.echo_optional_str_none(A22)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E22" s="2" t="e" cm="1">
+        <f t="array" ref="E22">_xll.echo_optional_str_list_none(A22)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="5">
         <f ca="1">TODAY()</f>
-        <v>45436</v>
+        <v>45469</v>
       </c>
       <c r="B23" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B23" ca="1">_xll.echo_type_datetime(A23)</f>
@@ -846,11 +988,19 @@
         <f t="array" aca="1" ref="C23" ca="1">_xll.echo_type_datetime_list(A23)</f>
         <v>&lt;class 'list'&gt;</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D23" s="2" cm="1">
+        <f t="array" aca="1" ref="D23" ca="1">_xll.echo_datetime(A23)</f>
+        <v>45444</v>
+      </c>
+      <c r="E23" s="2" cm="1">
+        <f t="array" aca="1" ref="E23" ca="1">_xll.echo_datetime_list(A23)</f>
+        <v>45444</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="5">
         <f t="shared" ref="A24:A26" ca="1" si="0">TODAY()</f>
-        <v>45436</v>
+        <v>45469</v>
       </c>
       <c r="B24" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B24" ca="1">_xll.echo_type_datetime_none(A24)</f>
@@ -860,11 +1010,19 @@
         <f t="array" aca="1" ref="C24" ca="1">_xll.echo_type_datetime_list_none(A24)</f>
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D24" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="D24" ca="1">_xll.echo_datetime_none(A24)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E24" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="E24" ca="1">_xll.echo_datetime_list_none(A24)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45436</v>
+        <v>45469</v>
       </c>
       <c r="B25" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B25" ca="1">_xll.echo_type_optional_datetime(A25)</f>
@@ -874,11 +1032,19 @@
         <f t="array" aca="1" ref="C25" ca="1">_xll.echo_type_optional_datetime_list(A25)</f>
         <v>&lt;class 'list'&gt;</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D25" s="2" cm="1">
+        <f t="array" aca="1" ref="D25" ca="1">_xll.echo_optional_datetime(A25)</f>
+        <v>45444</v>
+      </c>
+      <c r="E25" s="2" cm="1">
+        <f t="array" aca="1" ref="E25" ca="1">_xll.echo_optional_datetime_list(A25)</f>
+        <v>45444</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45436</v>
+        <v>45469</v>
       </c>
       <c r="B26" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B26" ca="1">_xll.echo_type_optional_datetime_none(A26)</f>
@@ -888,16 +1054,39 @@
         <f t="array" aca="1" ref="C26" ca="1">_xll.echo_type_optional_datetime_list_none(A26)</f>
         <v>&lt;class 'NoneType'&gt;</v>
       </c>
+      <c r="D26" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="D26" ca="1">_xll.echo_optional_datetime_none(A26)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E26" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="E26" ca="1">_xll.echo_optional_datetime_list_none(A26)</f>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E6:H8"/>
+    <mergeCell ref="I6:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056A28DAB99C48B469009752D21F8474A" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4c4b8f5646149e3f00102529456f19af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a" xmlns:ns4="03cbfcaa-e9f2-4603-927f-51e6fbd98e3f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8c990d4c29e86872f4a8caf520611414" ns3:_="" ns4:_="">
     <xsd:import namespace="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
@@ -1092,22 +1281,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20294D4-57D2-40C2-87DA-054488011DAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="03cbfcaa-e9f2-4603-927f-51e6fbd98e3f"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55E7368E-38DA-4735-83BC-E58CF361EF06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5BA672F-4AA7-448E-8867-6C159CA2ED93}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1124,29 +1323,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55E7368E-38DA-4735-83BC-E58CF361EF06}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20294D4-57D2-40C2-87DA-054488011DAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="03cbfcaa-e9f2-4603-927f-51e6fbd98e3f"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>